<commit_message>
added support for combining multiple results files and reanalyzing
</commit_message>
<xml_diff>
--- a/data/SPA52/Intensities.xlsx
+++ b/data/SPA52/Intensities.xlsx
@@ -7,16 +7,16 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Intensities" sheetId="1" r:id="rId1"/>
+    <sheet name="7184" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
   <si>
-    <t>Messpunkt</t>
+    <t>Cycle</t>
   </si>
   <si>
     <t>229Th</t>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>238U</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Error (%)</t>
   </si>
   <si>
     <t>[V]</t>
@@ -397,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I122"/>
+  <dimension ref="A1:I125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -406,12 +412,12 @@
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="19.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1">
@@ -445,28 +451,28 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1">
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -474,10 +480,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.03464730815879005</v>
+        <v>0.03466431211879036</v>
       </c>
       <c r="C3">
-        <v>0.03116235939276273</v>
+        <v>0.03116235799070553</v>
       </c>
       <c r="D3">
         <v>4.130224765528973</v>
@@ -503,10 +509,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.03455797535646329</v>
+        <v>0.03457491645747184</v>
       </c>
       <c r="C4">
-        <v>0.03115523318768577</v>
+        <v>0.03115523179081161</v>
       </c>
       <c r="D4">
         <v>4.134602097381928</v>
@@ -532,10 +538,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.03458245988375801</v>
+        <v>0.03459934017734666</v>
       </c>
       <c r="C5">
-        <v>0.0311437068258837</v>
+        <v>0.03114370543402339</v>
       </c>
       <c r="D5">
         <v>4.133433835111111</v>
@@ -561,10 +567,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.03459887536615937</v>
+        <v>0.03461584740725603</v>
       </c>
       <c r="C6">
-        <v>0.0312117464529453</v>
+        <v>0.03121174505351998</v>
       </c>
       <c r="D6">
         <v>4.13519985284635</v>
@@ -590,10 +596,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.03412347067219168</v>
+        <v>0.03414033791707465</v>
       </c>
       <c r="C7">
-        <v>0.0307097454800447</v>
+        <v>0.03070974408926032</v>
       </c>
       <c r="D7">
         <v>4.071816547142114</v>
@@ -619,10 +625,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.03416841818366918</v>
+        <v>0.03418536403614991</v>
       </c>
       <c r="C8">
-        <v>0.03071809649177426</v>
+        <v>0.03071809509450832</v>
       </c>
       <c r="D8">
         <v>4.086226589865451</v>
@@ -648,10 +654,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.03328995590340493</v>
+        <v>0.03330639617644077</v>
       </c>
       <c r="C9">
-        <v>0.02997386394111591</v>
+        <v>0.02997386258553739</v>
       </c>
       <c r="D9">
         <v>3.975962105206693</v>
@@ -677,10 +683,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.03338083193272989</v>
+        <v>0.0333971135422305</v>
       </c>
       <c r="C10">
-        <v>0.03002884178974538</v>
+        <v>0.03002884044724941</v>
       </c>
       <c r="D10">
         <v>3.983413649778368</v>
@@ -706,10 +712,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.03368593803283286</v>
+        <v>0.03370257037593373</v>
       </c>
       <c r="C11">
-        <v>0.0303572865916057</v>
+        <v>0.03035728522019009</v>
       </c>
       <c r="D11">
         <v>4.024104290471206</v>
@@ -735,10 +741,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.03296693396755844</v>
+        <v>0.03298315526467702</v>
       </c>
       <c r="C12">
-        <v>0.02974280750687686</v>
+        <v>0.02974280616935394</v>
       </c>
       <c r="D12">
         <v>3.946752271233882</v>
@@ -764,10 +770,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.03371737751899976</v>
+        <v>0.03373382367957855</v>
       </c>
       <c r="C13">
-        <v>0.03033865385510484</v>
+        <v>0.03033865249904086</v>
       </c>
       <c r="D13">
         <v>4.025967027813276</v>
@@ -793,10 +799,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.0333109574994983</v>
+        <v>0.03332729566458647</v>
       </c>
       <c r="C14">
-        <v>0.03001306616465357</v>
+        <v>0.03001306481749434</v>
       </c>
       <c r="D14">
         <v>3.977723575189047</v>
@@ -822,10 +828,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.03397782104391497</v>
+        <v>0.03399397383006181</v>
       </c>
       <c r="C15">
-        <v>0.03054306357884716</v>
+        <v>0.03054306224697329</v>
       </c>
       <c r="D15">
         <v>4.053920618181253</v>
@@ -851,10 +857,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.03450340042124819</v>
+        <v>0.03452025498914468</v>
       </c>
       <c r="C16">
-        <v>0.0311458572916375</v>
+        <v>0.0311458559018984</v>
       </c>
       <c r="D16">
         <v>4.122335924430836</v>
@@ -880,10 +886,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.03450048092022952</v>
+        <v>0.03451744765585841</v>
       </c>
       <c r="C17">
-        <v>0.031064275184413</v>
+        <v>0.03106427378542513</v>
       </c>
       <c r="D17">
         <v>4.12247534843362</v>
@@ -909,10 +915,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.03462957886726398</v>
+        <v>0.03464653749840475</v>
       </c>
       <c r="C18">
-        <v>0.03115710861505951</v>
+        <v>0.0311571072167399</v>
       </c>
       <c r="D18">
         <v>4.139355899448966</v>
@@ -938,10 +944,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.03447786545502309</v>
+        <v>0.03449477146075159</v>
       </c>
       <c r="C19">
-        <v>0.03108790299505454</v>
+        <v>0.03108790160107414</v>
       </c>
       <c r="D19">
         <v>4.122074770861789</v>
@@ -967,10 +973,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.0344192931864062</v>
+        <v>0.03443607284563618</v>
       </c>
       <c r="C20">
-        <v>0.03096343721908834</v>
+        <v>0.03096343583552582</v>
       </c>
       <c r="D20">
         <v>4.115197065229881</v>
@@ -996,10 +1002,10 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.03445958464181033</v>
+        <v>0.0344764512809139</v>
       </c>
       <c r="C21">
-        <v>0.03106171826678888</v>
+        <v>0.03106171687605445</v>
       </c>
       <c r="D21">
         <v>4.120832624544129</v>
@@ -1025,10 +1031,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.03389175972458946</v>
+        <v>0.03390854503803245</v>
       </c>
       <c r="C22">
-        <v>0.0305456669427317</v>
+        <v>0.03054566555870296</v>
       </c>
       <c r="D22">
         <v>4.049182816115196</v>
@@ -1054,10 +1060,10 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.03431673369498853</v>
+        <v>0.03433366205831823</v>
       </c>
       <c r="C23">
-        <v>0.03092272887952788</v>
+        <v>0.03092272748370399</v>
       </c>
       <c r="D23">
         <v>4.103127133582579</v>
@@ -1083,10 +1089,10 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.03420775518597246</v>
+        <v>0.03422467396230282</v>
       </c>
       <c r="C24">
-        <v>0.03086104651351825</v>
+        <v>0.03086104511848486</v>
       </c>
       <c r="D24">
         <v>4.091593882822411</v>
@@ -1112,10 +1118,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.03337791474401823</v>
+        <v>0.03339441162433173</v>
       </c>
       <c r="C25">
-        <v>0.03015793218904166</v>
+        <v>0.03015793082879559</v>
       </c>
       <c r="D25">
         <v>3.997091261595278</v>
@@ -1141,10 +1147,10 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.03428638945337853</v>
+        <v>0.03430327269180499</v>
       </c>
       <c r="C26">
-        <v>0.03092658317908552</v>
+        <v>0.0309265817869824</v>
       </c>
       <c r="D26">
         <v>4.100172769212172</v>
@@ -1170,10 +1176,10 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.03427798225196674</v>
+        <v>0.03429497123064688</v>
       </c>
       <c r="C27">
-        <v>0.03093201828679062</v>
+        <v>0.03093201688596871</v>
       </c>
       <c r="D27">
         <v>4.10173449844708</v>
@@ -1199,10 +1205,10 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.03446467660251581</v>
+        <v>0.03448152573290334</v>
       </c>
       <c r="C28">
-        <v>0.03103468142972632</v>
+        <v>0.03103468004043557</v>
       </c>
       <c r="D28">
         <v>4.119024505822702</v>
@@ -1228,10 +1234,10 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.03414418941810728</v>
+        <v>0.03416104147972402</v>
       </c>
       <c r="C29">
-        <v>0.03072361897395127</v>
+        <v>0.03072361758441882</v>
       </c>
       <c r="D29">
         <v>4.080057406509906</v>
@@ -1257,10 +1263,10 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.03399180654775803</v>
+        <v>0.03400850789708349</v>
       </c>
       <c r="C30">
-        <v>0.0305516515861839</v>
+        <v>0.03055165020907839</v>
       </c>
       <c r="D30">
         <v>4.063809974679342</v>
@@ -1286,10 +1292,10 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.0334367968197266</v>
+        <v>0.03345342086767428</v>
       </c>
       <c r="C31">
-        <v>0.03015081889143148</v>
+        <v>0.03015081752069985</v>
       </c>
       <c r="D31">
         <v>4.002031037630928</v>
@@ -1315,10 +1321,10 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.03322794626346055</v>
+        <v>0.03324443192933305</v>
       </c>
       <c r="C32">
-        <v>0.02997741800828841</v>
+        <v>0.02997741664896704</v>
       </c>
       <c r="D32">
         <v>3.968346827683009</v>
@@ -1344,10 +1350,10 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.03290526580857722</v>
+        <v>0.03292125651115393</v>
       </c>
       <c r="C33">
-        <v>0.02959951229392729</v>
+        <v>0.02959951097541798</v>
       </c>
       <c r="D33">
         <v>3.926454997881817</v>
@@ -1373,10 +1379,10 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.03392076645773334</v>
+        <v>0.03393718421145359</v>
       </c>
       <c r="C34">
-        <v>0.03062705233890424</v>
+        <v>0.03062705098518254</v>
       </c>
       <c r="D34">
         <v>4.061890055181673</v>
@@ -1402,10 +1408,10 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.03453678174298831</v>
+        <v>0.03455381250854572</v>
       </c>
       <c r="C35">
-        <v>0.03112336957544814</v>
+        <v>0.0311233681711807</v>
       </c>
       <c r="D35">
         <v>4.130803519117193</v>
@@ -1431,10 +1437,10 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.0346743651669179</v>
+        <v>0.03469125131042725</v>
       </c>
       <c r="C36">
-        <v>0.03118898379705969</v>
+        <v>0.03118898240471703</v>
       </c>
       <c r="D36">
         <v>4.144807454716625</v>
@@ -1460,10 +1466,10 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.03465801305639617</v>
+        <v>0.03467502893800858</v>
       </c>
       <c r="C37">
-        <v>0.03123833195328495</v>
+        <v>0.03123833055024477</v>
       </c>
       <c r="D37">
         <v>4.143575294780878</v>
@@ -1489,10 +1495,10 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.03443557086029162</v>
+        <v>0.03445249529147241</v>
       </c>
       <c r="C38">
-        <v>0.0309985160055776</v>
+        <v>0.03099851461007794</v>
       </c>
       <c r="D38">
         <v>4.116712556954088</v>
@@ -1518,10 +1524,10 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0.03435236836516653</v>
+        <v>0.03436939010642251</v>
       </c>
       <c r="C39">
-        <v>0.03100332167556858</v>
+        <v>0.03100332027204524</v>
       </c>
       <c r="D39">
         <v>4.110762646492361</v>
@@ -1547,10 +1553,10 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.03436268745139121</v>
+        <v>0.03437965890665544</v>
       </c>
       <c r="C40">
-        <v>0.03092726809368042</v>
+        <v>0.0309272666943034</v>
       </c>
       <c r="D40">
         <v>4.107375300682727</v>
@@ -1576,10 +1582,10 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.03419648466295</v>
+        <v>0.03421308838557816</v>
       </c>
       <c r="C41">
-        <v>0.03081586109286024</v>
+        <v>0.03081585972380453</v>
       </c>
       <c r="D41">
         <v>4.091971036844098</v>
@@ -1605,10 +1611,10 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>0.03414012714714877</v>
+        <v>0.03415708656415173</v>
       </c>
       <c r="C42">
-        <v>0.03076107198923156</v>
+        <v>0.03076107059084714</v>
       </c>
       <c r="D42">
         <v>4.084237681197657</v>
@@ -1634,10 +1640,10 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>0.03344369670545071</v>
+        <v>0.03346065081792472</v>
       </c>
       <c r="C43">
-        <v>0.03019912995330916</v>
+        <v>0.03019912855536213</v>
       </c>
       <c r="D43">
         <v>4.00616317101439</v>
@@ -1663,10 +1669,10 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>0.03415858181741215</v>
+        <v>0.03417533279090932</v>
       </c>
       <c r="C44">
-        <v>0.03082994210332472</v>
+        <v>0.03082994072212747</v>
       </c>
       <c r="D44">
         <v>4.086277887361516</v>
@@ -1692,10 +1698,10 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>0.0342630713925081</v>
+        <v>0.03428006809905027</v>
       </c>
       <c r="C45">
-        <v>0.03089626647062158</v>
+        <v>0.03089626506916248</v>
       </c>
       <c r="D45">
         <v>4.096160622008703</v>
@@ -1721,10 +1727,10 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>0.03457366992489171</v>
+        <v>0.03459073022721001</v>
       </c>
       <c r="C46">
-        <v>0.03112541158312437</v>
+        <v>0.03112541017642149</v>
       </c>
       <c r="D46">
         <v>4.134362519596056</v>
@@ -1750,10 +1756,10 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>0.03434444978487594</v>
+        <v>0.03436144056790658</v>
       </c>
       <c r="C47">
-        <v>0.03098287188720237</v>
+        <v>0.03098287048623168</v>
       </c>
       <c r="D47">
         <v>4.112125994428676</v>
@@ -1779,10 +1785,10 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>0.03434724262387723</v>
+        <v>0.03436408875082399</v>
       </c>
       <c r="C48">
-        <v>0.03091749878555576</v>
+        <v>0.03091749739651266</v>
       </c>
       <c r="D48">
         <v>4.105055273162353</v>
@@ -1808,10 +1814,10 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>0.03432161603969142</v>
+        <v>0.03433835384064041</v>
       </c>
       <c r="C49">
-        <v>0.03090254141429234</v>
+        <v>0.03090254003418123</v>
       </c>
       <c r="D49">
         <v>4.099372622685037</v>
@@ -1837,10 +1843,10 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>0.03442858524027564</v>
+        <v>0.03444552006531251</v>
       </c>
       <c r="C50">
-        <v>0.03098337564867208</v>
+        <v>0.03098337425231539</v>
       </c>
       <c r="D50">
         <v>4.115216535219197</v>
@@ -1866,10 +1872,10 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>0.03438056152403342</v>
+        <v>0.03439752468559872</v>
       </c>
       <c r="C51">
-        <v>0.03095581567161905</v>
+        <v>0.03095581427292588</v>
       </c>
       <c r="D51">
         <v>4.115313925153172</v>
@@ -1895,10 +1901,10 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>0.03425137282345647</v>
+        <v>0.03426834647674772</v>
       </c>
       <c r="C52">
-        <v>0.03087647536541042</v>
+        <v>0.03087647396585216</v>
       </c>
       <c r="D52">
         <v>4.096722925149907</v>
@@ -1924,10 +1930,10 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>0.03300914374003708</v>
+        <v>0.03302577683194842</v>
       </c>
       <c r="C53">
-        <v>0.02972965629603596</v>
+        <v>0.0297296549245586</v>
       </c>
       <c r="D53">
         <v>3.946513031664281</v>
@@ -1953,10 +1959,10 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>0.03405447043004635</v>
+        <v>0.03407145855239997</v>
       </c>
       <c r="C54">
-        <v>0.03069275416630544</v>
+        <v>0.03069275276555414</v>
       </c>
       <c r="D54">
         <v>4.074834174803962</v>
@@ -1982,10 +1988,10 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>0.03436892590393546</v>
+        <v>0.03438600085521016</v>
       </c>
       <c r="C55">
-        <v>0.03094837085322394</v>
+        <v>0.03094836944531318</v>
       </c>
       <c r="D55">
         <v>4.111311099897301</v>
@@ -2011,10 +2017,10 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>0.03416340176118171</v>
+        <v>0.0341804652051353</v>
       </c>
       <c r="C56">
-        <v>0.0308099694469637</v>
+        <v>0.03080996804000177</v>
       </c>
       <c r="D56">
         <v>4.089642387855477</v>
@@ -2040,10 +2046,10 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>0.03431054673038216</v>
+        <v>0.03432759158728258</v>
       </c>
       <c r="C57">
-        <v>0.03099264205638567</v>
+        <v>0.03099264065095634</v>
       </c>
       <c r="D57">
         <v>4.105482890048743</v>
@@ -2069,10 +2075,10 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>0.0343444775324669</v>
+        <v>0.03436152740579638</v>
       </c>
       <c r="C58">
-        <v>0.03092493019326867</v>
+        <v>0.03092492878742571</v>
       </c>
       <c r="D58">
         <v>4.102377058726657</v>
@@ -2098,10 +2104,10 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>0.03423173145785741</v>
+        <v>0.03424876779200017</v>
       </c>
       <c r="C59">
-        <v>0.03089190774626629</v>
+        <v>0.0308919063415397</v>
       </c>
       <c r="D59">
         <v>4.096104165576722</v>
@@ -2127,10 +2133,10 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>0.03423736743030097</v>
+        <v>0.03425444272692587</v>
       </c>
       <c r="C60">
-        <v>0.03085441301869886</v>
+        <v>0.03085441161075963</v>
       </c>
       <c r="D60">
         <v>4.095327458519828</v>
@@ -2156,10 +2162,10 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>0.0341575159694105</v>
+        <v>0.03417439253613554</v>
       </c>
       <c r="C61">
-        <v>0.03074998030410177</v>
+        <v>0.03074997891254877</v>
       </c>
       <c r="D61">
         <v>4.084015766593475</v>
@@ -2185,10 +2191,10 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>0.03404605437973838</v>
+        <v>0.03406305652742692</v>
       </c>
       <c r="C62">
-        <v>0.03069124827608592</v>
+        <v>0.03069124687417816</v>
       </c>
       <c r="D62">
         <v>4.074062055979115</v>
@@ -2214,10 +2220,10 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>0.03332343074736361</v>
+        <v>0.03333972191087754</v>
       </c>
       <c r="C63">
-        <v>0.02999597702322218</v>
+        <v>0.02999597567993845</v>
       </c>
       <c r="D63">
         <v>3.984069280466301</v>
@@ -2243,10 +2249,10 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>0.03432387334543091</v>
+        <v>0.03434093112093427</v>
       </c>
       <c r="C64">
-        <v>0.03092322393163773</v>
+        <v>0.0309232225251432</v>
       </c>
       <c r="D64">
         <v>4.102235747720094</v>
@@ -2272,10 +2278,10 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>0.03431627237477445</v>
+        <v>0.03433346369029615</v>
       </c>
       <c r="C65">
-        <v>0.03090121822240758</v>
+        <v>0.03090121680490204</v>
       </c>
       <c r="D65">
         <v>4.110039211334561</v>
@@ -2301,10 +2307,10 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>0.03458566938607081</v>
+        <v>0.0346028157722866</v>
       </c>
       <c r="C66">
-        <v>0.03116033152670436</v>
+        <v>0.03116033011290345</v>
       </c>
       <c r="D66">
         <v>4.134890109057647</v>
@@ -2330,10 +2336,10 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>0.03426103553161721</v>
+        <v>0.03427814112831126</v>
       </c>
       <c r="C67">
-        <v>0.0308005220434037</v>
+        <v>0.03080052063296609</v>
       </c>
       <c r="D67">
         <v>4.094710474774418</v>
@@ -2359,10 +2365,10 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>0.03448313923232439</v>
+        <v>0.03450024348857043</v>
       </c>
       <c r="C68">
-        <v>0.03099760483691795</v>
+        <v>0.03099760342659087</v>
       </c>
       <c r="D68">
         <v>4.124350371899682</v>
@@ -2388,10 +2394,10 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>0.03434989214351123</v>
+        <v>0.03436697358174019</v>
       </c>
       <c r="C69">
-        <v>0.03098651086787455</v>
+        <v>0.03098650945942891</v>
       </c>
       <c r="D69">
         <v>4.104961994256285</v>
@@ -2417,10 +2423,10 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>0.0344289935079824</v>
+        <v>0.0344461800742361</v>
       </c>
       <c r="C70">
-        <v>0.03102659454447559</v>
+        <v>0.03102659312736164</v>
       </c>
       <c r="D70">
         <v>4.120980782136611</v>
@@ -2446,10 +2452,10 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>0.03441017692291868</v>
+        <v>0.03442727050332808</v>
       </c>
       <c r="C71">
-        <v>0.0309153935842701</v>
+        <v>0.03091539217482328</v>
       </c>
       <c r="D71">
         <v>4.110508130307483</v>
@@ -2475,10 +2481,10 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>0.0340320800135786</v>
+        <v>0.03404923124884933</v>
       </c>
       <c r="C72">
-        <v>0.03061793127840568</v>
+        <v>0.03061792986420495</v>
       </c>
       <c r="D72">
         <v>4.071394064866965</v>
@@ -2504,10 +2510,10 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>0.03389878645367266</v>
+        <v>0.03391519706878259</v>
       </c>
       <c r="C73">
-        <v>0.03045463703548561</v>
+        <v>0.03045463568235252</v>
       </c>
       <c r="D73">
         <v>4.047853584885599</v>
@@ -2533,10 +2539,10 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>0.03437257890168642</v>
+        <v>0.0343895567659169</v>
       </c>
       <c r="C74">
-        <v>0.03094309951422865</v>
+        <v>0.03094309811432318</v>
       </c>
       <c r="D74">
         <v>4.105539719940731</v>
@@ -2562,10 +2568,10 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>0.03432084031080224</v>
+        <v>0.03433790949027581</v>
       </c>
       <c r="C75">
-        <v>0.03084274705263498</v>
+        <v>0.03084274564520014</v>
       </c>
       <c r="D75">
         <v>4.100247024038524</v>
@@ -2591,10 +2597,10 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>0.03435825790760998</v>
+        <v>0.03437536011398581</v>
       </c>
       <c r="C76">
-        <v>0.03094137050048042</v>
+        <v>0.03094136909032235</v>
       </c>
       <c r="D76">
         <v>4.110691998050698</v>
@@ -2620,10 +2626,10 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>0.03445806948759296</v>
+        <v>0.03447511381890724</v>
       </c>
       <c r="C77">
-        <v>0.03102305093528188</v>
+        <v>0.03102304952989589</v>
       </c>
       <c r="D77">
         <v>4.11298959388254</v>
@@ -2649,10 +2655,10 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>0.03386160921525037</v>
+        <v>0.03387847735599434</v>
       </c>
       <c r="C78">
-        <v>0.03047607761223583</v>
+        <v>0.03047607622137759</v>
       </c>
       <c r="D78">
         <v>4.046960808435219</v>
@@ -2678,10 +2684,10 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>0.0341786823039009</v>
+        <v>0.03419572843786729</v>
       </c>
       <c r="C79">
-        <v>0.03077275924802984</v>
+        <v>0.03077275784249521</v>
       </c>
       <c r="D79">
         <v>4.085595645369727</v>
@@ -2707,10 +2713,10 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>0.03436893143091106</v>
+        <v>0.03438610513445208</v>
       </c>
       <c r="C80">
-        <v>0.03099707514601334</v>
+        <v>0.03099707372995999</v>
       </c>
       <c r="D80">
         <v>4.109391665009936</v>
@@ -2736,10 +2742,10 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>0.03440649027903105</v>
+        <v>0.03442368263003662</v>
       </c>
       <c r="C81">
-        <v>0.03096912099958145</v>
+        <v>0.03096911958199053</v>
       </c>
       <c r="D81">
         <v>4.112312434938665</v>
@@ -2765,10 +2771,10 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>0.03340403799431337</v>
+        <v>0.0334211198644721</v>
       </c>
       <c r="C82">
-        <v>0.02998771478263886</v>
+        <v>0.02998771337415761</v>
       </c>
       <c r="D82">
         <v>3.993533511472144</v>
@@ -2794,10 +2800,10 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>0.03421188798937257</v>
+        <v>0.03422868230287706</v>
       </c>
       <c r="C83">
-        <v>0.03073184326245307</v>
+        <v>0.03073184187768222</v>
       </c>
       <c r="D83">
         <v>4.087072931665434</v>
@@ -2823,10 +2829,10 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>0.03432572308497255</v>
+        <v>0.03434286244447896</v>
       </c>
       <c r="C84">
-        <v>0.03101141125959848</v>
+        <v>0.03101140984637697</v>
       </c>
       <c r="D84">
         <v>4.109807839497862</v>
@@ -2852,10 +2858,10 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>0.03440352094715189</v>
+        <v>0.03442055411258217</v>
       </c>
       <c r="C85">
-        <v>0.03095306633384049</v>
+        <v>0.03095306492937518</v>
       </c>
       <c r="D85">
         <v>4.113129741015132</v>
@@ -2881,10 +2887,10 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>0.0342513349611117</v>
+        <v>0.03426849920001016</v>
       </c>
       <c r="C86">
-        <v>0.03083219768882152</v>
+        <v>0.03083219627354858</v>
       </c>
       <c r="D86">
         <v>4.094436287552174</v>
@@ -2910,10 +2916,10 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>0.0337358751572274</v>
+        <v>0.03375309124681924</v>
       </c>
       <c r="C87">
-        <v>0.03040138664846311</v>
+        <v>0.03040138522891483</v>
       </c>
       <c r="D87">
         <v>4.044089415999923</v>
@@ -2939,10 +2945,10 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>0.03433104792954237</v>
+        <v>0.03434823724817212</v>
       </c>
       <c r="C88">
-        <v>0.03092912800685123</v>
+        <v>0.03092912658951034</v>
       </c>
       <c r="D88">
         <v>4.107966316696023</v>
@@ -2968,10 +2974,10 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>0.03437970869990241</v>
+        <v>0.03439695170565964</v>
       </c>
       <c r="C89">
-        <v>0.03099614813563386</v>
+        <v>0.03099614671386621</v>
       </c>
       <c r="D89">
         <v>4.113405896748137</v>
@@ -2997,10 +3003,10 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>0.03423134116133121</v>
+        <v>0.03424856635722526</v>
       </c>
       <c r="C90">
-        <v>0.03081331004266213</v>
+        <v>0.03081330862236299</v>
       </c>
       <c r="D90">
         <v>4.088388157059121</v>
@@ -3026,10 +3032,10 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>0.03372649873202327</v>
+        <v>0.03374368932362648</v>
       </c>
       <c r="C91">
-        <v>0.03037709807096519</v>
+        <v>0.03037709665351934</v>
       </c>
       <c r="D91">
         <v>4.040283989939858</v>
@@ -3055,10 +3061,10 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>0.0343209365803919</v>
+        <v>0.03433763663440584</v>
       </c>
       <c r="C92">
-        <v>0.03086020791995004</v>
+        <v>0.03086020654295134</v>
       </c>
       <c r="D92">
         <v>4.103378085715816</v>
@@ -3084,10 +3090,10 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>0.03439366522864663</v>
+        <v>0.03441076139154926</v>
       </c>
       <c r="C93">
-        <v>0.03104526608220821</v>
+        <v>0.03104526467254845</v>
       </c>
       <c r="D93">
         <v>4.120665599905262</v>
@@ -3113,10 +3119,10 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>0.03446592110427727</v>
+        <v>0.0344831890283621</v>
       </c>
       <c r="C94">
-        <v>0.03104625966952222</v>
+        <v>0.03104625824569994</v>
       </c>
       <c r="D94">
         <v>4.118160249753448</v>
@@ -3142,10 +3148,10 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>0.03438825317103019</v>
+        <v>0.03440538202633751</v>
       </c>
       <c r="C95">
-        <v>0.03089135659632448</v>
+        <v>0.03089135518396908</v>
       </c>
       <c r="D95">
         <v>4.10758495330531</v>
@@ -3171,10 +3177,10 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>0.03445990802599559</v>
+        <v>0.03447713063562717</v>
       </c>
       <c r="C96">
-        <v>0.0310367718127032</v>
+        <v>0.03103677039261732</v>
       </c>
       <c r="D96">
         <v>4.123043036574712</v>
@@ -3200,10 +3206,10 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>0.03443564401244308</v>
+        <v>0.03445279554884191</v>
       </c>
       <c r="C97">
-        <v>0.03101004484461102</v>
+        <v>0.03101004343038546</v>
       </c>
       <c r="D97">
         <v>4.110939244079085</v>
@@ -3229,10 +3235,10 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>0.03411235844076794</v>
+        <v>0.03412954793099207</v>
       </c>
       <c r="C98">
-        <v>0.03078926235930945</v>
+        <v>0.03078926094195441</v>
       </c>
       <c r="D98">
         <v>4.085788035831741</v>
@@ -3258,10 +3264,10 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>0.03422687880698844</v>
+        <v>0.03424409483385083</v>
       </c>
       <c r="C99">
-        <v>0.030812607393759</v>
+        <v>0.03081260597421589</v>
       </c>
       <c r="D99">
         <v>4.094719102353155</v>
@@ -3287,10 +3293,10 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>0.03427812324327383</v>
+        <v>0.03429545862480213</v>
       </c>
       <c r="C100">
-        <v>0.03080987037244054</v>
+        <v>0.03080986894305608</v>
       </c>
       <c r="D100">
         <v>4.096655277422865</v>
@@ -3316,10 +3322,10 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>0.03317704191301126</v>
+        <v>0.03319391780877901</v>
       </c>
       <c r="C101">
-        <v>0.02988105487577349</v>
+        <v>0.0298810534842758</v>
       </c>
       <c r="D101">
         <v>3.967231194048563</v>
@@ -3345,10 +3351,10 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>0.03446303798745842</v>
+        <v>0.03448012451386698</v>
       </c>
       <c r="C102">
-        <v>0.03101451334840792</v>
+        <v>0.03101451193954273</v>
       </c>
       <c r="D102">
         <v>4.121237660485345</v>
@@ -3374,10 +3380,10 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>0.03427388950913769</v>
+        <v>0.03429110131886495</v>
       </c>
       <c r="C103">
-        <v>0.03085835658183647</v>
+        <v>0.03085835516264109</v>
       </c>
       <c r="D103">
         <v>4.097921617499913</v>
@@ -3403,10 +3409,10 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>0.03430633369390185</v>
+        <v>0.03432359088914524</v>
       </c>
       <c r="C104">
-        <v>0.03085183087381632</v>
+        <v>0.03085182945087868</v>
       </c>
       <c r="D104">
         <v>4.101565768976774</v>
@@ -3432,10 +3438,10 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>0.03451330389837563</v>
+        <v>0.03453053146711173</v>
       </c>
       <c r="C105">
-        <v>0.0310090463568189</v>
+        <v>0.03100904493632411</v>
       </c>
       <c r="D105">
         <v>4.124955230330623</v>
@@ -3461,10 +3467,10 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>0.03437490729628676</v>
+        <v>0.03439207400176347</v>
       </c>
       <c r="C106">
-        <v>0.03099718729961039</v>
+        <v>0.03099718588413407</v>
       </c>
       <c r="D106">
         <v>4.112915383532041</v>
@@ -3490,10 +3496,10 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>0.03401995443117638</v>
+        <v>0.03403729685370877</v>
       </c>
       <c r="C107">
-        <v>0.0306730003005919</v>
+        <v>0.03067299887062687</v>
       </c>
       <c r="D107">
         <v>4.073144450855718</v>
@@ -3519,10 +3525,10 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>0.03424811253476664</v>
+        <v>0.03426536990550347</v>
       </c>
       <c r="C108">
-        <v>0.03082863325737901</v>
+        <v>0.0308286318344269</v>
       </c>
       <c r="D108">
         <v>4.096033831044839</v>
@@ -3548,10 +3554,10 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>0.03442080443451184</v>
+        <v>0.0344380205148306</v>
       </c>
       <c r="C109">
-        <v>0.03095617084136427</v>
+        <v>0.03095616942181676</v>
       </c>
       <c r="D109">
         <v>4.117124021937367</v>
@@ -3577,10 +3583,10 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>0.03373294362001308</v>
+        <v>0.03375014981236202</v>
       </c>
       <c r="C110">
-        <v>0.03034982013883637</v>
+        <v>0.03034981872010416</v>
       </c>
       <c r="D110">
         <v>4.033848045582355</v>
@@ -3606,10 +3612,10 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>0.03404708306978874</v>
+        <v>0.03406359649807525</v>
       </c>
       <c r="C111">
-        <v>0.03064129729024951</v>
+        <v>0.03064129592863899</v>
       </c>
       <c r="D111">
         <v>4.069849836062193</v>
@@ -3635,10 +3641,10 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>0.03455463287433993</v>
+        <v>0.03457189002584717</v>
       </c>
       <c r="C112">
-        <v>0.0311484151638431</v>
+        <v>0.03114841374090907</v>
       </c>
       <c r="D112">
         <v>4.133801720446445</v>
@@ -3664,10 +3670,10 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>0.03464503593407638</v>
+        <v>0.03466231120816154</v>
       </c>
       <c r="C113">
-        <v>0.03116822021307944</v>
+        <v>0.03116821878865113</v>
       </c>
       <c r="D113">
         <v>4.138523310586233</v>
@@ -3693,10 +3699,10 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>0.03445274955099985</v>
+        <v>0.03447012978565712</v>
       </c>
       <c r="C114">
-        <v>0.03098637934849872</v>
+        <v>0.03098637791541591</v>
       </c>
       <c r="D114">
         <v>4.117596585141829</v>
@@ -3722,10 +3728,10 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>0.03436955712466108</v>
+        <v>0.03438693350879735</v>
       </c>
       <c r="C115">
-        <v>0.03097736949394259</v>
+        <v>0.03097736806117726</v>
       </c>
       <c r="D115">
         <v>4.111094490053421</v>
@@ -3751,10 +3757,10 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>0.03443580990677466</v>
+        <v>0.0344531524897515</v>
       </c>
       <c r="C116">
-        <v>0.03104016450195784</v>
+        <v>0.03104016307197958</v>
       </c>
       <c r="D116">
         <v>4.115443998171854</v>
@@ -3780,10 +3786,10 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>0.03433102481975937</v>
+        <v>0.0343484442182281</v>
       </c>
       <c r="C117">
-        <v>0.03087709659258668</v>
+        <v>0.03087709515627462</v>
       </c>
       <c r="D117">
         <v>4.104948266484315</v>
@@ -3809,10 +3815,10 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>0.03427005396477058</v>
+        <v>0.03428737565326884</v>
       </c>
       <c r="C118">
-        <v>0.03092419184606996</v>
+        <v>0.03092419041781454</v>
       </c>
       <c r="D118">
         <v>4.102673193109449</v>
@@ -3838,10 +3844,10 @@
         <v>117</v>
       </c>
       <c r="B119">
-        <v>0.03412223292718496</v>
+        <v>0.03413962345248776</v>
       </c>
       <c r="C119">
-        <v>0.03080405535016093</v>
+        <v>0.0308040539162296</v>
       </c>
       <c r="D119">
         <v>4.092667853312537</v>
@@ -3867,10 +3873,10 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>0.03328569790923739</v>
+        <v>0.03330279956397984</v>
       </c>
       <c r="C120">
-        <v>0.02999842877982337</v>
+        <v>0.02999842736971078</v>
       </c>
       <c r="D120">
         <v>3.984398682717214</v>
@@ -3896,10 +3902,10 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>0.0341254008278114</v>
+        <v>0.0341426233594113</v>
       </c>
       <c r="C121">
-        <v>0.03079258700937875</v>
+        <v>0.03079258558929929</v>
       </c>
       <c r="D121">
         <v>4.083952062565315</v>
@@ -3925,10 +3931,10 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>0.03429703239364408</v>
+        <v>0.03431451251850306</v>
       </c>
       <c r="C122">
-        <v>0.03096049476355453</v>
+        <v>0.0309604933222353</v>
       </c>
       <c r="D122">
         <v>4.103419076557702</v>
@@ -3947,6 +3953,64 @@
       </c>
       <c r="I122">
         <v>320.8216658266513</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
+      <c r="A124" t="s">
+        <v>9</v>
+      </c>
+      <c r="B124">
+        <v>0.03434189678270662</v>
+      </c>
+      <c r="C124">
+        <v>0.03092419041781454</v>
+      </c>
+      <c r="D124">
+        <v>4.1049551303703</v>
+      </c>
+      <c r="E124">
+        <v>0.009468819415328655</v>
+      </c>
+      <c r="F124">
+        <v>0.01732631144542124</v>
+      </c>
+      <c r="G124">
+        <v>2.247922296592716</v>
+      </c>
+      <c r="H124">
+        <v>1.155958434243606</v>
+      </c>
+      <c r="I124">
+        <v>312.8445891818169</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
+      <c r="A125" t="s">
+        <v>10</v>
+      </c>
+      <c r="B125">
+        <v>0.1227432499413368</v>
+      </c>
+      <c r="C125">
+        <v>0.1304131742577663</v>
+      </c>
+      <c r="D125">
+        <v>0.1206992037843743</v>
+      </c>
+      <c r="E125">
+        <v>0.2382916233479211</v>
+      </c>
+      <c r="F125">
+        <v>0.227718175066942</v>
+      </c>
+      <c r="G125">
+        <v>0.227159256936122</v>
+      </c>
+      <c r="H125">
+        <v>0.2277511178406862</v>
+      </c>
+      <c r="I125">
+        <v>0.2289579177964268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>